<commit_message>
data processing sequence done
</commit_message>
<xml_diff>
--- a/RuthWeek11/Requests/Requests.xlsx
+++ b/RuthWeek11/Requests/Requests.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>ContactName</t>
   </si>
@@ -25,13 +25,22 @@
     <t>Subject</t>
   </si>
   <si>
-    <t>Ruth</t>
-  </si>
-  <si>
-    <t>rmwangi2@gmail.com</t>
-  </si>
-  <si>
-    <t>email change</t>
+    <t>Account Name</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Account creation</t>
+  </si>
+  <si>
+    <t>Rose</t>
+  </si>
+  <si>
+    <t>Rose Mwangi</t>
+  </si>
+  <si>
+    <t>rm.4@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -384,14 +393,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.140625" customWidth="1"/>
     <col min="3" max="3" width="21" bestFit="1" customWidth="1"/>
   </cols>
@@ -401,7 +411,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -409,7 +419,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -418,6 +428,22 @@
       </c>
       <c r="B3" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>727290683</v>
       </c>
     </row>
   </sheetData>

</xml_diff>